<commit_message>
Small changes after first test
</commit_message>
<xml_diff>
--- a/input_files/EN18218_age_data.xlsx
+++ b/input_files/EN18218_age_data.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="8616" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="8616"/>
   </bookViews>
   <sheets>
     <sheet name="Age" sheetId="1" r:id="rId1"/>
@@ -502,8 +502,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M27"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C26" sqref="C26"/>
+    <sheetView tabSelected="1" topLeftCell="F4" workbookViewId="0">
+      <selection activeCell="M24" sqref="M24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -584,10 +584,10 @@
         <v>16</v>
       </c>
       <c r="L2" s="2">
-        <v>0</v>
+        <v>853</v>
       </c>
       <c r="M2" s="2">
-        <v>0</v>
+        <v>31</v>
       </c>
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.3">
@@ -625,10 +625,10 @@
         <v>16</v>
       </c>
       <c r="L3" s="2">
-        <v>0</v>
+        <v>853</v>
       </c>
       <c r="M3" s="2">
-        <v>0</v>
+        <v>31</v>
       </c>
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.3">
@@ -666,10 +666,10 @@
         <v>16</v>
       </c>
       <c r="L4" s="2">
-        <v>0</v>
+        <v>853</v>
       </c>
       <c r="M4" s="2">
-        <v>0</v>
+        <v>31</v>
       </c>
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.3">
@@ -707,10 +707,10 @@
         <v>16</v>
       </c>
       <c r="L5" s="2">
-        <v>0</v>
+        <v>853</v>
       </c>
       <c r="M5" s="2">
-        <v>0</v>
+        <v>31</v>
       </c>
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.3">
@@ -748,10 +748,10 @@
         <v>16</v>
       </c>
       <c r="L6" s="2">
-        <v>0</v>
+        <v>853</v>
       </c>
       <c r="M6" s="2">
-        <v>0</v>
+        <v>31</v>
       </c>
     </row>
     <row r="7" spans="1:13" x14ac:dyDescent="0.3">
@@ -789,10 +789,10 @@
         <v>16</v>
       </c>
       <c r="L7" s="2">
-        <v>0</v>
+        <v>853</v>
       </c>
       <c r="M7" s="2">
-        <v>0</v>
+        <v>31</v>
       </c>
     </row>
     <row r="8" spans="1:13" x14ac:dyDescent="0.3">
@@ -830,10 +830,10 @@
         <v>16</v>
       </c>
       <c r="L8" s="2">
-        <v>0</v>
+        <v>853</v>
       </c>
       <c r="M8" s="2">
-        <v>0</v>
+        <v>31</v>
       </c>
     </row>
     <row r="9" spans="1:13" x14ac:dyDescent="0.3">
@@ -871,10 +871,10 @@
         <v>16</v>
       </c>
       <c r="L9" s="2">
-        <v>0</v>
+        <v>853</v>
       </c>
       <c r="M9" s="2">
-        <v>0</v>
+        <v>31</v>
       </c>
     </row>
     <row r="10" spans="1:13" x14ac:dyDescent="0.3">
@@ -912,10 +912,10 @@
         <v>16</v>
       </c>
       <c r="L10" s="2">
-        <v>0</v>
+        <v>853</v>
       </c>
       <c r="M10" s="2">
-        <v>0</v>
+        <v>31</v>
       </c>
     </row>
     <row r="11" spans="1:13" x14ac:dyDescent="0.3">
@@ -953,10 +953,10 @@
         <v>16</v>
       </c>
       <c r="L11" s="2">
-        <v>0</v>
+        <v>853</v>
       </c>
       <c r="M11" s="2">
-        <v>0</v>
+        <v>31</v>
       </c>
     </row>
     <row r="12" spans="1:13" x14ac:dyDescent="0.3">
@@ -994,10 +994,10 @@
         <v>16</v>
       </c>
       <c r="L12" s="2">
-        <v>0</v>
+        <v>853</v>
       </c>
       <c r="M12" s="2">
-        <v>0</v>
+        <v>31</v>
       </c>
     </row>
     <row r="13" spans="1:13" x14ac:dyDescent="0.3">
@@ -1035,10 +1035,10 @@
         <v>16</v>
       </c>
       <c r="L13" s="2">
-        <v>0</v>
+        <v>853</v>
       </c>
       <c r="M13" s="2">
-        <v>0</v>
+        <v>31</v>
       </c>
     </row>
     <row r="14" spans="1:13" x14ac:dyDescent="0.3">
@@ -1076,10 +1076,10 @@
         <v>16</v>
       </c>
       <c r="L14" s="2">
-        <v>0</v>
+        <v>853</v>
       </c>
       <c r="M14" s="2">
-        <v>0</v>
+        <v>31</v>
       </c>
     </row>
     <row r="15" spans="1:13" x14ac:dyDescent="0.3">
@@ -1117,10 +1117,10 @@
         <v>16</v>
       </c>
       <c r="L15" s="2">
-        <v>0</v>
+        <v>853</v>
       </c>
       <c r="M15" s="2">
-        <v>0</v>
+        <v>31</v>
       </c>
     </row>
     <row r="16" spans="1:13" x14ac:dyDescent="0.3">
@@ -1158,10 +1158,10 @@
         <v>16</v>
       </c>
       <c r="L16" s="2">
-        <v>0</v>
+        <v>853</v>
       </c>
       <c r="M16" s="2">
-        <v>0</v>
+        <v>31</v>
       </c>
     </row>
     <row r="17" spans="1:13" x14ac:dyDescent="0.3">
@@ -1199,10 +1199,10 @@
         <v>16</v>
       </c>
       <c r="L17" s="2">
-        <v>0</v>
+        <v>853</v>
       </c>
       <c r="M17" s="2">
-        <v>0</v>
+        <v>31</v>
       </c>
     </row>
     <row r="18" spans="1:13" x14ac:dyDescent="0.3">
@@ -1240,10 +1240,10 @@
         <v>16</v>
       </c>
       <c r="L18" s="2">
-        <v>0</v>
+        <v>853</v>
       </c>
       <c r="M18" s="2">
-        <v>0</v>
+        <v>31</v>
       </c>
     </row>
     <row r="19" spans="1:13" x14ac:dyDescent="0.3">
@@ -1281,10 +1281,10 @@
         <v>16</v>
       </c>
       <c r="L19" s="2">
-        <v>0</v>
+        <v>853</v>
       </c>
       <c r="M19" s="2">
-        <v>0</v>
+        <v>31</v>
       </c>
     </row>
     <row r="20" spans="1:13" x14ac:dyDescent="0.3">
@@ -1322,10 +1322,10 @@
         <v>16</v>
       </c>
       <c r="L20" s="2">
-        <v>0</v>
+        <v>853</v>
       </c>
       <c r="M20" s="2">
-        <v>0</v>
+        <v>31</v>
       </c>
     </row>
     <row r="21" spans="1:13" x14ac:dyDescent="0.3">
@@ -1363,10 +1363,10 @@
         <v>16</v>
       </c>
       <c r="L21" s="2">
-        <v>0</v>
+        <v>853</v>
       </c>
       <c r="M21" s="2">
-        <v>0</v>
+        <v>31</v>
       </c>
     </row>
     <row r="22" spans="1:13" x14ac:dyDescent="0.3">
@@ -1404,10 +1404,10 @@
         <v>16</v>
       </c>
       <c r="L22" s="2">
-        <v>0</v>
+        <v>853</v>
       </c>
       <c r="M22" s="2">
-        <v>0</v>
+        <v>31</v>
       </c>
     </row>
     <row r="23" spans="1:13" x14ac:dyDescent="0.3">
@@ -1445,10 +1445,10 @@
         <v>16</v>
       </c>
       <c r="L23" s="2">
-        <v>0</v>
+        <v>853</v>
       </c>
       <c r="M23" s="2">
-        <v>0</v>
+        <v>31</v>
       </c>
     </row>
     <row r="24" spans="1:13" x14ac:dyDescent="0.3">
@@ -1486,10 +1486,10 @@
         <v>16</v>
       </c>
       <c r="L24" s="2">
-        <v>0</v>
+        <v>853</v>
       </c>
       <c r="M24" s="2">
-        <v>0</v>
+        <v>31</v>
       </c>
     </row>
     <row r="25" spans="1:13" x14ac:dyDescent="0.3">
@@ -1527,10 +1527,10 @@
         <v>16</v>
       </c>
       <c r="L25" s="2">
-        <v>0</v>
+        <v>853</v>
       </c>
       <c r="M25" s="2">
-        <v>0</v>
+        <v>31</v>
       </c>
     </row>
     <row r="26" spans="1:13" x14ac:dyDescent="0.3">
@@ -1568,10 +1568,10 @@
         <v>16</v>
       </c>
       <c r="L26" s="2">
-        <v>0</v>
+        <v>853</v>
       </c>
       <c r="M26" s="2">
-        <v>0</v>
+        <v>31</v>
       </c>
     </row>
     <row r="27" spans="1:13" x14ac:dyDescent="0.3">
@@ -1609,10 +1609,10 @@
         <v>16</v>
       </c>
       <c r="L27" s="2">
-        <v>0</v>
+        <v>853</v>
       </c>
       <c r="M27" s="2">
-        <v>0</v>
+        <v>31</v>
       </c>
     </row>
   </sheetData>
@@ -1624,7 +1624,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>

</xml_diff>